<commit_message>
Investigate what is happening at the end of the REGEX
</commit_message>
<xml_diff>
--- a/Excel_Challenge_608 - Extract Zip and Country.xlsx
+++ b/Excel_Challenge_608 - Extract Zip and Country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680C51C4-AA89-4374-9D05-017BB0B58200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A643A05-3752-42BA-B484-844E78E255EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -152,14 +152,26 @@
     <t>Wrong Zip Codes in Two Locations</t>
   </si>
   <si>
-    <t>My Single Function</t>
+    <t>My Single Function (With Correct Zip Codes)</t>
+  </si>
+  <si>
+    <t>Why is the lookahead at the end needed?</t>
+  </si>
+  <si>
+    <t>A simple grab of the first result</t>
+  </si>
+  <si>
+    <t>The REGEX is returning two cells</t>
+  </si>
+  <si>
+    <t>Are there trailing spaces?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +186,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF7030A0"/>
+      <name val="Aptos Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -205,10 +232,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -223,8 +252,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comment" xfId="2" xr:uid="{6FE6F66E-CB93-4D3C-8060-931457AD3CB8}"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -829,10 +862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0A282D-0783-4A1A-A38F-B0C02B4FAB7F}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1121,10 +1154,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F14" t="s">
+      <c r="F14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1333,6 +1366,289 @@
       </c>
       <c r="O24" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F28" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F30" t="str" cm="1">
+        <f t="array" ref="F30">_xlfn.REGEXEXTRACT(A3,"[A-Za-z]*$",0)</f>
+        <v>Germany</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <f>COLUMNS(_xlfn.REGEXEXTRACT(A3,"[A-Za-z]*$",1))</f>
+        <v>2</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F32" t="str" cm="1">
+        <f t="array" ref="F32:G32">_xlfn.REGEXEXTRACT(A9,"[A-Za-z]*$",1)</f>
+        <v>Kingdom</v>
+      </c>
+      <c r="G32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="L35" t="str" cm="1">
+        <f t="array" ref="L35:L44">MID(G32,_xlfn.SEQUENCE(10,1,1,1),1)</f>
+        <v/>
+      </c>
+      <c r="M35" t="e">
+        <f>CODE(L35)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="36" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I36" t="str" cm="1">
+        <f t="array" ref="I36:I55">MID(A4,LEN(A4)-_xlfn.SEQUENCE(20,1,12,-1),1)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J36">
+        <f>CODE(I36)</f>
+        <v>32</v>
+      </c>
+      <c r="L36" t="str">
+        <v/>
+      </c>
+      <c r="M36" t="e">
+        <f t="shared" ref="M36:M44" si="0">CODE(L36)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="37" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I37" t="str">
+        <v>T</v>
+      </c>
+      <c r="J37">
+        <f t="shared" ref="J37:J52" si="1">CODE(I37)</f>
+        <v>84</v>
+      </c>
+      <c r="L37" t="str">
+        <v/>
+      </c>
+      <c r="M37" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="38" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I38" t="str">
+        <v>a</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="L38" t="str">
+        <v/>
+      </c>
+      <c r="M38" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="39" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I39" t="str">
+        <v>n</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="L39" t="str">
+        <v/>
+      </c>
+      <c r="M39" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="40" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I40" t="str">
+        <v>a</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="L40" t="str">
+        <v/>
+      </c>
+      <c r="M40" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="41" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I41" t="str">
+        <v>k</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="L41" t="str">
+        <v/>
+      </c>
+      <c r="M41" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="42" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I42" t="str">
+        <v>a</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="L42" t="str">
+        <v/>
+      </c>
+      <c r="M42" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="43" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I43" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="L43" t="str">
+        <v/>
+      </c>
+      <c r="M43" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="44" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I44" t="str">
+        <v>J</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="L44" t="str">
+        <v/>
+      </c>
+      <c r="M44" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="45" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I45" t="str">
+        <v>a</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I46" t="str">
+        <v>p</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I47" t="str">
+        <v>a</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I48" t="str">
+        <v>n</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="I49" t="str">
+        <v/>
+      </c>
+      <c r="J49" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="I50" t="str">
+        <v/>
+      </c>
+      <c r="J50" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="51" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="I51" t="str">
+        <v/>
+      </c>
+      <c r="J51" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="52" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="I52" t="str">
+        <v/>
+      </c>
+      <c r="J52" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="53" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="I53" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="I54" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F55" t="str" cm="1">
+        <f t="array" ref="F55">_xlfn.REGEXEXTRACT(A3,"[A-Za-z]+$",1)</f>
+        <v>Germany</v>
+      </c>
+      <c r="I55" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I got a simple REGEX working
</commit_message>
<xml_diff>
--- a/Excel_Challenge_608 - Extract Zip and Country.xlsx
+++ b/Excel_Challenge_608 - Extract Zip and Country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A643A05-3752-42BA-B484-844E78E255EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF877785-B25E-4435-9C09-F07E5A538962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="36">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Are there trailing spaces?</t>
+  </si>
+  <si>
+    <t>I can make a simple REGEX (no lookahead) work</t>
   </si>
 </sst>
 </file>
@@ -862,10 +865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0A282D-0783-4A1A-A38F-B0C02B4FAB7F}">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1643,12 +1646,73 @@
       </c>
     </row>
     <row r="55" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F55" t="str" cm="1">
-        <f t="array" ref="F55">_xlfn.REGEXEXTRACT(A3,"[A-Za-z]+$",1)</f>
-        <v>Germany</v>
-      </c>
       <c r="I55" t="str">
         <v/>
+      </c>
+    </row>
+    <row r="56" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F56" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F57" t="str" cm="1">
+        <f t="array" ref="F57">_xlfn.REGEXEXTRACT(A3,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="58" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F58" t="str" cm="1">
+        <f t="array" ref="F58">_xlfn.REGEXEXTRACT(A4,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>Japan</v>
+      </c>
+    </row>
+    <row r="59" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F59" t="str" cm="1">
+        <f t="array" ref="F59">_xlfn.REGEXEXTRACT(A5,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>Canada</v>
+      </c>
+    </row>
+    <row r="60" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F60" t="str" cm="1">
+        <f t="array" ref="F60">_xlfn.REGEXEXTRACT(A6,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="61" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F61" t="str" cm="1">
+        <f t="array" ref="F61">_xlfn.REGEXEXTRACT(A7,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>Australia</v>
+      </c>
+    </row>
+    <row r="62" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F62" t="str" cm="1">
+        <f t="array" ref="F62">_xlfn.REGEXEXTRACT(A8,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>France</v>
+      </c>
+    </row>
+    <row r="63" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F63" t="str" cm="1">
+        <f t="array" ref="F63">_xlfn.REGEXEXTRACT(A9,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>United Kingdom</v>
+      </c>
+    </row>
+    <row r="64" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F64" t="str" cm="1">
+        <f t="array" ref="F64">_xlfn.REGEXEXTRACT(A10,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>Brazil</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F65" t="str" cm="1">
+        <f t="array" ref="F65">_xlfn.REGEXEXTRACT(A11,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>United States</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F66" t="str" cm="1">
+        <f t="array" ref="F66">_xlfn.REGEXEXTRACT(A12,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>New Zealand</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I think I finally understand what is going on
</commit_message>
<xml_diff>
--- a/Excel_Challenge_608 - Extract Zip and Country.xlsx
+++ b/Excel_Challenge_608 - Extract Zip and Country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF877785-B25E-4435-9C09-F07E5A538962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B45DE60-7BF7-467E-8583-FD8944402976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>I can make a simple REGEX (no lookahead) work</t>
+  </si>
+  <si>
+    <t>Using a 0 or more (*) operator results in two matches and the function showed the last one, which was empty.</t>
+  </si>
+  <si>
+    <t>Why was there an an empty match? It was an option that was TRUE. Using the + operator removed the empty option.</t>
+  </si>
+  <si>
+    <t>Alternate Formula Form</t>
   </si>
 </sst>
 </file>
@@ -865,10 +874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0A282D-0783-4A1A-A38F-B0C02B4FAB7F}">
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,6 +885,7 @@
     <col min="1" max="1" width="56.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="12" max="12" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1656,63 +1666,223 @@
       </c>
     </row>
     <row r="57" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F57" t="str" cm="1">
-        <f t="array" ref="F57">_xlfn.REGEXEXTRACT(A3,"(United |New )?[A-Za-z]+$",1)</f>
-        <v>Germany</v>
-      </c>
+      <c r="F57" s="8"/>
     </row>
     <row r="58" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F58" t="str" cm="1">
-        <f t="array" ref="F58">_xlfn.REGEXEXTRACT(A4,"(United |New )?[A-Za-z]+$",1)</f>
-        <v>Japan</v>
+        <f t="array" ref="F58">_xlfn.REGEXEXTRACT(A3,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>Germany</v>
       </c>
     </row>
     <row r="59" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F59" t="str" cm="1">
-        <f t="array" ref="F59">_xlfn.REGEXEXTRACT(A5,"(United |New )?[A-Za-z]+$",1)</f>
-        <v>Canada</v>
+        <f t="array" ref="F59">_xlfn.REGEXEXTRACT(A4,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>Japan</v>
       </c>
     </row>
     <row r="60" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F60" t="str" cm="1">
-        <f t="array" ref="F60">_xlfn.REGEXEXTRACT(A6,"(United |New )?[A-Za-z]+$",1)</f>
-        <v>India</v>
+        <f t="array" ref="F60">_xlfn.REGEXEXTRACT(A5,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>Canada</v>
       </c>
     </row>
     <row r="61" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F61" t="str" cm="1">
-        <f t="array" ref="F61">_xlfn.REGEXEXTRACT(A7,"(United |New )?[A-Za-z]+$",1)</f>
-        <v>Australia</v>
+        <f t="array" ref="F61">_xlfn.REGEXEXTRACT(A6,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>India</v>
       </c>
     </row>
     <row r="62" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F62" t="str" cm="1">
-        <f t="array" ref="F62">_xlfn.REGEXEXTRACT(A8,"(United |New )?[A-Za-z]+$",1)</f>
-        <v>France</v>
+        <f t="array" ref="F62">_xlfn.REGEXEXTRACT(A7,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>Australia</v>
       </c>
     </row>
     <row r="63" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F63" t="str" cm="1">
-        <f t="array" ref="F63">_xlfn.REGEXEXTRACT(A9,"(United |New )?[A-Za-z]+$",1)</f>
-        <v>United Kingdom</v>
+        <f t="array" ref="F63">_xlfn.REGEXEXTRACT(A8,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>France</v>
       </c>
     </row>
     <row r="64" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F64" t="str" cm="1">
-        <f t="array" ref="F64">_xlfn.REGEXEXTRACT(A10,"(United |New )?[A-Za-z]+$",1)</f>
+        <f t="array" ref="F64">_xlfn.REGEXEXTRACT(A9,"(United |New )?[A-Za-z]+$",1)</f>
+        <v>United Kingdom</v>
+      </c>
+    </row>
+    <row r="65" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F65" t="str" cm="1">
+        <f t="array" ref="F65">_xlfn.REGEXEXTRACT(A10,"(United |New )?[A-Za-z]+$",1)</f>
         <v>Brazil</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F65" t="str" cm="1">
-        <f t="array" ref="F65">_xlfn.REGEXEXTRACT(A11,"(United |New )?[A-Za-z]+$",1)</f>
+    <row r="66" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F66" t="str" cm="1">
+        <f t="array" ref="F66">_xlfn.REGEXEXTRACT(A11,"(United |New )?[A-Za-z]+$",1)</f>
         <v>United States</v>
       </c>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F66" t="str" cm="1">
-        <f t="array" ref="F66">_xlfn.REGEXEXTRACT(A12,"(United |New )?[A-Za-z]+$",1)</f>
+    <row r="67" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F67" t="str" cm="1">
+        <f t="array" ref="F67">_xlfn.REGEXEXTRACT(A12,"(United |New )?[A-Za-z]+$",1)</f>
         <v>New Zealand</v>
+      </c>
+    </row>
+    <row r="69" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F69" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F70" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F72" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F74" cm="1">
+        <f t="array" ref="F74:G83">_xlfn.HSTACK(0+_xlfn.DROP(_xlfn.REDUCE("",A3:A12, _xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TAKE(_xlfn.REGEXEXTRACT(_xlpm.v,"\d{5,6}",1),,-1)))),1),TRIM(_xlfn.REGEXEXTRACT(A3:A12,"(United |New )?[A-Za-z]+$",1)))</f>
+        <v>98765</v>
+      </c>
+      <c r="G74" t="str">
+        <v>Germany</v>
+      </c>
+      <c r="I74" t="b" cm="1">
+        <f t="array" ref="I74:J83">_xlfn.ANCHORARRAY(F74)=B3:C12</f>
+        <v>1</v>
+      </c>
+      <c r="J74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <v>10293</v>
+      </c>
+      <c r="G75" t="str">
+        <v>Japan</v>
+      </c>
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
+      <c r="J75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F76">
+        <v>54321</v>
+      </c>
+      <c r="G76" t="str">
+        <v>Canada</v>
+      </c>
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+      <c r="J76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F77">
+        <v>400001</v>
+      </c>
+      <c r="G77" t="str">
+        <v>India</v>
+      </c>
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
+      <c r="J77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F78">
+        <v>56789</v>
+      </c>
+      <c r="G78" t="str">
+        <v>Australia</v>
+      </c>
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
+      <c r="J78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F79">
+        <v>75001</v>
+      </c>
+      <c r="G79" t="str">
+        <v>France</v>
+      </c>
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+      <c r="J79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F80">
+        <v>65432</v>
+      </c>
+      <c r="G80" t="str">
+        <v>United Kingdom</v>
+      </c>
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+      <c r="J80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F81">
+        <v>85247</v>
+      </c>
+      <c r="G81" t="str">
+        <v>Brazil</v>
+      </c>
+      <c r="I81" t="b">
+        <v>1</v>
+      </c>
+      <c r="J81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <v>12345</v>
+      </c>
+      <c r="G82" t="str">
+        <v>United States</v>
+      </c>
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F83">
+        <v>36987</v>
+      </c>
+      <c r="G83" t="str">
+        <v>New Zealand</v>
+      </c>
+      <c r="I83" t="b">
+        <v>1</v>
+      </c>
+      <c r="J83" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recorded some final observations
</commit_message>
<xml_diff>
--- a/Excel_Challenge_608 - Extract Zip and Country.xlsx
+++ b/Excel_Challenge_608 - Extract Zip and Country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B45DE60-7BF7-467E-8583-FD8944402976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE4E2D2-5ADE-4CE7-88BC-3207CA9B71A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>Alternate Formula Form</t>
+  </si>
+  <si>
+    <t>The key point here is that if your regex only returns one item, you can just pass it an array of addresses. However, if the regex returns more than 1, you must stack</t>
+  </si>
+  <si>
+    <t>the data in a REDUCE.</t>
   </si>
 </sst>
 </file>
@@ -721,6 +727,35 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="222" row="9">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{F3BB0D08-F24C-426B-A4BB-FABC0C178FB5}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{92AF05ED-74F5-458D-ADA2-305E68CBBA47}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
@@ -874,10 +909,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0A282D-0783-4A1A-A38F-B0C02B4FAB7F}">
-  <dimension ref="A1:O83"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="B70" workbookViewId="0">
+      <selection activeCell="O73" sqref="O73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1745,7 +1780,18 @@
     </row>
     <row r="74" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F74" cm="1">
-        <f t="array" ref="F74:G83">_xlfn.HSTACK(0+_xlfn.DROP(_xlfn.REDUCE("",A3:A12, _xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TAKE(_xlfn.REGEXEXTRACT(_xlpm.v,"\d{5,6}",1),,-1)))),1),TRIM(_xlfn.REGEXEXTRACT(A3:A12,"(United |New )?[A-Za-z]+$",1)))</f>
+        <f t="array" ref="F74:G83">_xlfn.HSTACK(
+    0 +
+        _xlfn.DROP(
+            _xlfn.REDUCE(
+                "",
+                A3:A12,
+                _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlfn.TAKE(_xlfn.REGEXEXTRACT(_xlpm.v, "\d{5,6}", 1), , -1)))
+            ),
+            1
+        ),
+    TRIM(_xlfn.REGEXEXTRACT(A3:A12, "(United |New )?[A-Za-z]+$", 1))
+)</f>
         <v>98765</v>
       </c>
       <c r="G74" t="str">
@@ -1883,6 +1929,16 @@
       </c>
       <c r="J83" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F85" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F86" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2130,4 +2186,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92AF05ED-74F5-458D-ADA2-305E68CBBA47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>